<commit_message>
Added condorcet and a few helper functions. Made some code to also generate a heatmap of conditions that generate a condorcet winner.
</commit_message>
<xml_diff>
--- a/Heat Map for Likelyhood of Condorcet Winners.xlsx
+++ b/Heat Map for Likelyhood of Condorcet Winners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josh/Desktop/Math and Democracy/VotingSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7726DCDD-06F4-4443-A2CD-2B814AA07BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F604E-0197-DA41-B01C-2EC2E47A1349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8388643A-C411-144B-86AF-0B6149320FC0}"/>
   </bookViews>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>How many candidates, below. How many voters, to the right.</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -388,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEBC72F-AD24-FD4D-BD9A-0DCDBDA32513}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="91" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,7 +411,7 @@
         <v>20</v>
       </c>
       <c r="D1">
-        <f t="shared" ref="D1:T1" si="0">C1+10</f>
+        <f t="shared" ref="D1:U1" si="0">C1+10</f>
         <v>30</v>
       </c>
       <c r="E1">
@@ -475,8 +478,12 @@
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U1">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -537,8 +544,11 @@
       <c r="T2">
         <v>0.95699999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U2">
+        <v>0.93799999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -599,8 +609,11 @@
       <c r="T3">
         <v>0.81599999999999995</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U3">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -661,8 +674,11 @@
       <c r="T4">
         <v>0.72499999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U4">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -723,8 +739,11 @@
       <c r="T5">
         <v>0.63300000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="U5">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -776,9 +795,948 @@
       <c r="Q6">
         <v>0.58699999999999997</v>
       </c>
+      <c r="R6">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="S6">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="T6">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="U6">
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.42</v>
+      </c>
+      <c r="E7">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="F7">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="J7">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="K7">
+        <v>0.52</v>
+      </c>
+      <c r="L7">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="M7">
+        <v>0.48</v>
+      </c>
+      <c r="N7">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="O7">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="P7">
+        <v>0.495</v>
+      </c>
+      <c r="Q7">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="R7">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="S7">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="T7">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="U7">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="F8">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="H8">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="I8">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="J8">
+        <v>0.433</v>
+      </c>
+      <c r="K8">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="L8">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="M8">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="N8">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="O8">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="P8">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="Q8">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="R8">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="S8">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="T8">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="U8">
+        <v>0.49399999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.26</v>
+      </c>
+      <c r="C9">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.318</v>
+      </c>
+      <c r="E9">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="F9">
+        <v>0.36</v>
+      </c>
+      <c r="G9">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.432</v>
+      </c>
+      <c r="K9">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="L9">
+        <v>0.433</v>
+      </c>
+      <c r="M9">
+        <v>0.441</v>
+      </c>
+      <c r="N9">
+        <v>0.432</v>
+      </c>
+      <c r="O9">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="P9">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="Q9">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="R9">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="S9">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="T9">
+        <v>0.442</v>
+      </c>
+      <c r="U9">
+        <v>0.46100000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E10">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="H10">
+        <v>0.372</v>
+      </c>
+      <c r="I10">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.36</v>
+      </c>
+      <c r="K10">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="L10">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="M10">
+        <v>0.39</v>
+      </c>
+      <c r="N10">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="O10">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="P10">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="Q10">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="R10">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="S10">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="T10">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="U10">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.249</v>
+      </c>
+      <c r="D11">
+        <v>0.26</v>
+      </c>
+      <c r="E11">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.313</v>
+      </c>
+      <c r="H11">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="I11">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="J11">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.375</v>
+      </c>
+      <c r="L11">
+        <v>0.371</v>
+      </c>
+      <c r="M11">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="N11">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="O11">
+        <v>0.35</v>
+      </c>
+      <c r="P11">
+        <v>0.376</v>
+      </c>
+      <c r="Q11">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="R11">
+        <v>0.376</v>
+      </c>
+      <c r="S11">
+        <v>0.37</v>
+      </c>
+      <c r="T11">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="U11">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="E12">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.317</v>
+      </c>
+      <c r="H12">
+        <v>0.31</v>
+      </c>
+      <c r="I12">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="J12">
+        <v>0.3</v>
+      </c>
+      <c r="K12">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="L12">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="M12">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="N12">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="O12">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="P12">
+        <v>0.35</v>
+      </c>
+      <c r="Q12">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="R12">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="S12">
+        <v>0.379</v>
+      </c>
+      <c r="T12">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="U12">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="C13">
+        <v>0.218</v>
+      </c>
+      <c r="D13">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.255</v>
+      </c>
+      <c r="F13">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="H13">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="J13">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.32</v>
+      </c>
+      <c r="L13">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="M13">
+        <v>0.314</v>
+      </c>
+      <c r="N13">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="O13">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="P13">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="Q13">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="R13">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="S13">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="T13">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="U13">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.151</v>
+      </c>
+      <c r="C14">
+        <v>0.183</v>
+      </c>
+      <c r="D14">
+        <v>0.25</v>
+      </c>
+      <c r="E14">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.247</v>
+      </c>
+      <c r="G14">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="H14">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="I14">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="J14">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K14">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="L14">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="M14">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="N14">
+        <v>0.312</v>
+      </c>
+      <c r="O14">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="P14">
+        <v>0.32</v>
+      </c>
+      <c r="Q14">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="R14">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="S14">
+        <v>0.311</v>
+      </c>
+      <c r="T14">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="U14">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.128</v>
+      </c>
+      <c r="C15">
+        <v>0.189</v>
+      </c>
+      <c r="D15">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="H15">
+        <v>0.254</v>
+      </c>
+      <c r="I15">
+        <v>0.24</v>
+      </c>
+      <c r="J15">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="K15">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="L15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="M15">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="N15">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="O15">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="P15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="Q15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="R15">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="S15">
+        <v>0.3</v>
+      </c>
+      <c r="T15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="U15">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.22</v>
+      </c>
+      <c r="E16">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.248</v>
+      </c>
+      <c r="H16">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="I16">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="J16">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="K16">
+        <v>0.255</v>
+      </c>
+      <c r="L16">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="M16">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="N16">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="O16">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="P16">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="Q16">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="R16">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="S16">
+        <v>0.318</v>
+      </c>
+      <c r="T16">
+        <v>0.317</v>
+      </c>
+      <c r="U16">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.121</v>
+      </c>
+      <c r="C17">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.191</v>
+      </c>
+      <c r="E17">
+        <v>0.184</v>
+      </c>
+      <c r="F17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="G17">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="H17">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="I17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="J17">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="K17">
+        <v>0.246</v>
+      </c>
+      <c r="L17">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="M17">
+        <v>0.247</v>
+      </c>
+      <c r="N17">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="P17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q17">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="R17">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="S17">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="T17">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="U17">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="C18">
+        <v>0.151</v>
+      </c>
+      <c r="D18">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F18">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H18">
+        <v>0.245</v>
+      </c>
+      <c r="I18">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="J18">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="K18">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="L18">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="M18">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="N18">
+        <v>0.223</v>
+      </c>
+      <c r="O18">
+        <v>0.246</v>
+      </c>
+      <c r="P18">
+        <v>0.247</v>
+      </c>
+      <c r="Q18">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="R18">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="S18">
+        <v>0.255</v>
+      </c>
+      <c r="T18">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="U18">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>0.115</v>
+      </c>
+      <c r="C19">
+        <v>0.159</v>
+      </c>
+      <c r="D19">
+        <v>0.189</v>
+      </c>
+      <c r="E19">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.223</v>
+      </c>
+      <c r="G19">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H19">
+        <v>0.245</v>
+      </c>
+      <c r="I19">
+        <v>0.218</v>
+      </c>
+      <c r="J19">
+        <v>0.223</v>
+      </c>
+      <c r="K19">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="L19">
+        <v>0.253</v>
+      </c>
+      <c r="M19">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="N19">
+        <v>0.251</v>
+      </c>
+      <c r="O19">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="P19">
+        <v>0.249</v>
+      </c>
+      <c r="Q19">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="R19">
+        <v>0.224</v>
+      </c>
+      <c r="S19">
+        <v>0.253</v>
+      </c>
+      <c r="T19">
+        <v>0.24</v>
+      </c>
+      <c r="U19">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>0.107</v>
+      </c>
+      <c r="C20">
+        <v>0.129</v>
+      </c>
+      <c r="D20">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="E20">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="H20">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="I20">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="J20">
+        <v>0.21</v>
+      </c>
+      <c r="K20">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="L20">
+        <v>0.222</v>
+      </c>
+      <c r="M20">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="N20">
+        <v>0.21</v>
+      </c>
+      <c r="O20">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="P20">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>0.246</v>
+      </c>
+      <c r="R20">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="S20">
+        <v>0.248</v>
+      </c>
+      <c r="T20">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="U20">
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U21" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:T19">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:U20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Cleaned up the code and finished my heat map
</commit_message>
<xml_diff>
--- a/Heat Map for Likelyhood of Condorcet Winners.xlsx
+++ b/Heat Map for Likelyhood of Condorcet Winners.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josh/Desktop/Math and Democracy/VotingSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F604E-0197-DA41-B01C-2EC2E47A1349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D352DBCE-61FA-E24F-AAE4-06842B9E54B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8388643A-C411-144B-86AF-0B6149320FC0}"/>
   </bookViews>
@@ -393,11 +393,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BEBC72F-AD24-FD4D-BD9A-0DCDBDA32513}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="91" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="21" width="6.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>